<commit_message>
add device info get cmd
</commit_message>
<xml_diff>
--- a/zlg iot link protocol.xlsx
+++ b/zlg iot link protocol.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E5A59F-6018-4C38-9759-484AB2D98AB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A11C0E-C7C4-4056-B61C-B6E8973C34C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Link Protocol" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="236">
   <si>
     <t>帧头</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -706,23 +706,7 @@
     <t>PacketType Name</t>
   </si>
   <si>
-    <t>0x5A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Dev ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status Report</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0xB4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CMD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -764,6 +748,218 @@
   </si>
   <si>
     <t xml:space="preserve">                    TBD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果通讯链路不支持点对点通讯，则DevID被使用，否则保持为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NotificationReport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ErrorReport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetBatteryPercentage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xC0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notification
+Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LockType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KeyID (12 Bytes)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TamperAlarm/防撬报警</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KeyDeletedNotification/删除钥匙通知</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KeyAddedNotification/添加钥匙通知</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LowElectricityAlarm/低电量报警</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HijackingAlarm/劫持报警</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DoorUnlockedAlarm/门未锁好报警</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KeyInformationNotification/钥匙信息上报</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetKeyList/获取钥匙列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeleteKey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddKey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetKeyList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x5A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xB1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crc16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>length in bytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Report
+Packet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alarm
+Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xE0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DoorOpenNotification/开门通知</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电机故障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1</t>
+  </si>
+  <si>
+    <t>GetProductKey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetProductSecret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetDeviceName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetDeviceSecret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetAppVersion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetLockStat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x27</t>
+  </si>
+  <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>GetDeviceInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xnn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeviceInfoResponse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x82</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -846,7 +1042,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -978,11 +1174,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1055,8 +1297,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1064,14 +1324,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1088,14 +1372,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1377,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y75"/>
+  <dimension ref="A1:Y98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="D40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1400,11 +1687,11 @@
     <col min="13" max="13" width="7.6640625" customWidth="1"/>
     <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.109375" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.6640625" customWidth="1"/>
     <col min="18" max="18" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="22" width="10" customWidth="1"/>
-    <col min="23" max="23" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="63.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="25.77734375" customWidth="1"/>
     <col min="25" max="25" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1417,103 +1704,103 @@
       <c r="R2" s="22"/>
     </row>
     <row r="3" spans="1:25" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="32"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="32"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29" t="s">
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29" t="s">
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="33" t="s">
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="52"/>
+      <c r="W4" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="X4" s="33" t="s">
+      <c r="X4" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="Y4" s="33" t="s">
+      <c r="Y4" s="47" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28" t="s">
+      <c r="I5" s="51"/>
+      <c r="J5" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28" t="s">
+      <c r="K5" s="51"/>
+      <c r="L5" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="28"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
-      <c r="Y5" s="34"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
     </row>
     <row r="6" spans="1:25" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
@@ -1576,12 +1863,12 @@
       <c r="V6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
     </row>
     <row r="7" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="36" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1642,7 +1929,7 @@
       <c r="X7" s="16"/>
     </row>
     <row r="8" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="27"/>
+      <c r="C8" s="36"/>
       <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1701,7 +1988,7 @@
       <c r="X8" s="16"/>
     </row>
     <row r="9" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="27"/>
+      <c r="C9" s="36"/>
       <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1760,7 +2047,7 @@
       <c r="X9" s="16"/>
     </row>
     <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="27"/>
+      <c r="C10" s="36"/>
       <c r="E10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1819,7 +2106,7 @@
       <c r="X10" s="16"/>
     </row>
     <row r="11" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="27"/>
+      <c r="C11" s="36"/>
       <c r="E11" s="1" t="s">
         <v>31</v>
       </c>
@@ -1878,7 +2165,7 @@
       <c r="X11" s="16"/>
     </row>
     <row r="12" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="27"/>
+      <c r="C12" s="36"/>
       <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1888,32 +2175,32 @@
       <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36" t="s">
+      <c r="I12" s="50"/>
+      <c r="J12" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36" t="s">
+      <c r="K12" s="50"/>
+      <c r="L12" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="36"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
       <c r="W12" s="16"/>
       <c r="X12" s="16"/>
     </row>
     <row r="13" spans="1:25" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C13" s="27"/>
+      <c r="C13" s="36"/>
       <c r="E13" s="14" t="s">
         <v>32</v>
       </c>
@@ -1972,8 +2259,8 @@
       <c r="X13" s="16"/>
     </row>
     <row r="14" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="27"/>
-      <c r="D14" s="30" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="38" t="s">
         <v>72</v>
       </c>
       <c r="E14" s="13" t="s">
@@ -2024,8 +2311,8 @@
       <c r="X14" s="17"/>
     </row>
     <row r="15" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="27"/>
-      <c r="D15" s="30"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="13" t="s">
         <v>85</v>
       </c>
@@ -2070,8 +2357,8 @@
       <c r="X15" s="17"/>
     </row>
     <row r="16" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="27"/>
-      <c r="D16" s="30"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="13" t="s">
         <v>86</v>
       </c>
@@ -2116,8 +2403,8 @@
       <c r="X16" s="17"/>
     </row>
     <row r="17" spans="3:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="27"/>
-      <c r="D17" s="30"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="13" t="s">
         <v>87</v>
       </c>
@@ -2162,8 +2449,8 @@
       <c r="X17" s="17"/>
     </row>
     <row r="18" spans="3:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="27"/>
-      <c r="D18" s="30"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="13" t="s">
         <v>88</v>
       </c>
@@ -2208,8 +2495,8 @@
       <c r="X18" s="17"/>
     </row>
     <row r="19" spans="3:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="27"/>
-      <c r="D19" s="30"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="1" t="s">
         <v>89</v>
       </c>
@@ -2254,8 +2541,8 @@
       <c r="X19" s="17"/>
     </row>
     <row r="20" spans="3:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="27"/>
-      <c r="D20" s="30"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="11" t="s">
         <v>90</v>
       </c>
@@ -2300,8 +2587,8 @@
       <c r="X20" s="17"/>
     </row>
     <row r="21" spans="3:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="27"/>
-      <c r="D21" s="30"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="13" t="s">
         <v>103</v>
       </c>
@@ -2348,8 +2635,8 @@
       <c r="X21" s="17"/>
     </row>
     <row r="22" spans="3:25" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="27"/>
-      <c r="D22" s="30"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="13" t="s">
         <v>92</v>
       </c>
@@ -2388,8 +2675,8 @@
       <c r="X22" s="17"/>
     </row>
     <row r="23" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C23" s="27"/>
-      <c r="D23" s="30"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="12" t="s">
         <v>94</v>
       </c>
@@ -2428,8 +2715,8 @@
       <c r="X23" s="17"/>
     </row>
     <row r="24" spans="3:25" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="27"/>
-      <c r="D24" s="30"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="13" t="s">
         <v>95</v>
       </c>
@@ -2474,8 +2761,8 @@
       <c r="X24" s="17"/>
     </row>
     <row r="25" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C25" s="27"/>
-      <c r="D25" s="30"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="10" t="s">
         <v>96</v>
       </c>
@@ -2522,8 +2809,8 @@
       <c r="X25" s="16"/>
     </row>
     <row r="26" spans="3:25" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="27"/>
-      <c r="D26" s="30"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="38"/>
       <c r="E26" s="1" t="s">
         <v>97</v>
       </c>
@@ -2570,8 +2857,8 @@
       <c r="X26" s="16"/>
     </row>
     <row r="27" spans="3:25" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="27"/>
-      <c r="D27" s="30"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="38"/>
       <c r="E27" s="1" t="s">
         <v>98</v>
       </c>
@@ -2618,8 +2905,8 @@
       <c r="X27" s="16"/>
     </row>
     <row r="28" spans="3:25" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="27"/>
-      <c r="D28" s="30"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="1" t="s">
         <v>99</v>
       </c>
@@ -2666,8 +2953,8 @@
       <c r="X28" s="16"/>
     </row>
     <row r="29" spans="3:25" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="27"/>
-      <c r="D29" s="30"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="38"/>
       <c r="E29" s="1" t="s">
         <v>93</v>
       </c>
@@ -2711,8 +2998,8 @@
       </c>
     </row>
     <row r="30" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C30" s="27"/>
-      <c r="D30" s="30"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="38"/>
       <c r="E30" s="10" t="s">
         <v>101</v>
       </c>
@@ -2757,8 +3044,8 @@
       <c r="X30" s="16"/>
     </row>
     <row r="31" spans="3:25" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="27"/>
-      <c r="D31" s="30"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="38"/>
       <c r="E31" s="1" t="s">
         <v>100</v>
       </c>
@@ -2805,8 +3092,8 @@
       <c r="X31" s="16"/>
     </row>
     <row r="32" spans="3:25" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="27"/>
-      <c r="D32" s="30"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="1" t="s">
         <v>91</v>
       </c>
@@ -2834,9 +3121,9 @@
       <c r="W32" s="16"/>
       <c r="X32" s="16"/>
     </row>
-    <row r="33" spans="3:24" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="27"/>
-      <c r="D33" s="30"/>
+    <row r="33" spans="3:25" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="36"/>
+      <c r="D33" s="38"/>
       <c r="E33" s="1" t="s">
         <v>91</v>
       </c>
@@ -2864,9 +3151,9 @@
       <c r="W33" s="16"/>
       <c r="X33" s="16"/>
     </row>
-    <row r="34" spans="3:24" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="27"/>
-      <c r="D34" s="30"/>
+    <row r="34" spans="3:25" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="36"/>
+      <c r="D34" s="38"/>
       <c r="E34" s="10" t="s">
         <v>102</v>
       </c>
@@ -2904,8 +3191,8 @@
       <c r="W34" s="16"/>
       <c r="X34" s="16"/>
     </row>
-    <row r="35" spans="3:24" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C35" s="27"/>
+    <row r="35" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C35" s="36"/>
       <c r="E35" s="1"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2949,9 +3236,9 @@
       <c r="W35" s="16"/>
       <c r="X35" s="16"/>
     </row>
-    <row r="36" spans="3:24" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C36" s="27"/>
-      <c r="D36" s="30" t="s">
+    <row r="36" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C36" s="36"/>
+      <c r="D36" s="38" t="s">
         <v>71</v>
       </c>
       <c r="E36" s="13" t="s">
@@ -2989,9 +3276,9 @@
       <c r="W36" s="16"/>
       <c r="X36" s="16"/>
     </row>
-    <row r="37" spans="3:24" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C37" s="27"/>
-      <c r="D37" s="30"/>
+    <row r="37" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C37" s="36"/>
+      <c r="D37" s="38"/>
       <c r="E37" s="13" t="s">
         <v>79</v>
       </c>
@@ -3027,9 +3314,9 @@
       <c r="W37" s="16"/>
       <c r="X37" s="16"/>
     </row>
-    <row r="38" spans="3:24" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C38" s="27"/>
-      <c r="D38" s="30"/>
+    <row r="38" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C38" s="36"/>
+      <c r="D38" s="38"/>
       <c r="E38" s="13" t="s">
         <v>81</v>
       </c>
@@ -3055,19 +3342,19 @@
       <c r="Q38" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="R38" s="30" t="s">
+      <c r="R38" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="U38" s="27"/>
-      <c r="V38" s="27"/>
+      <c r="S38" s="36"/>
+      <c r="T38" s="36"/>
+      <c r="U38" s="36"/>
+      <c r="V38" s="36"/>
       <c r="W38" s="16"/>
       <c r="X38" s="16"/>
     </row>
-    <row r="39" spans="3:24" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C39" s="27"/>
-      <c r="D39" s="30"/>
+    <row r="39" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C39" s="36"/>
+      <c r="D39" s="38"/>
       <c r="E39" s="13" t="s">
         <v>82</v>
       </c>
@@ -3093,19 +3380,19 @@
       <c r="Q39" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="R39" s="27" t="s">
+      <c r="R39" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="S39" s="27"/>
-      <c r="T39" s="27"/>
-      <c r="U39" s="27"/>
-      <c r="V39" s="27"/>
+      <c r="S39" s="36"/>
+      <c r="T39" s="36"/>
+      <c r="U39" s="36"/>
+      <c r="V39" s="36"/>
       <c r="W39" s="16"/>
       <c r="X39" s="16"/>
     </row>
-    <row r="40" spans="3:24" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C40" s="27"/>
-      <c r="D40" s="30"/>
+    <row r="40" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C40" s="36"/>
+      <c r="D40" s="38"/>
       <c r="E40" s="1" t="s">
         <v>83</v>
       </c>
@@ -3141,9 +3428,9 @@
       <c r="W40" s="16"/>
       <c r="X40" s="16"/>
     </row>
-    <row r="41" spans="3:24" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="C41" s="27"/>
-      <c r="D41" s="31"/>
+    <row r="41" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C41" s="36"/>
+      <c r="D41" s="42"/>
       <c r="E41" s="13" t="s">
         <v>108</v>
       </c>
@@ -3179,7 +3466,7 @@
       <c r="W41" s="16"/>
       <c r="X41" s="16"/>
     </row>
-    <row r="42" spans="3:24" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:25" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="7" t="s">
         <v>34</v>
       </c>
@@ -3196,10 +3483,10 @@
         <v>3</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J42" s="24" t="s">
         <v>7</v>
@@ -3214,7 +3501,7 @@
         <v>17</v>
       </c>
       <c r="N42" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O42" s="8" t="s">
         <v>19</v>
@@ -3243,24 +3530,24 @@
       <c r="W42" s="16"/>
       <c r="X42" s="16"/>
     </row>
-    <row r="43" spans="3:24" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="38" t="s">
-        <v>185</v>
+    <row r="43" spans="3:25" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="37" t="s">
+        <v>181</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="I43" s="20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -3276,22 +3563,22 @@
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
     </row>
-    <row r="44" spans="3:24" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="27"/>
+    <row r="44" spans="3:25" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="36"/>
       <c r="E44" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H44" s="20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I44" s="20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
@@ -3307,30 +3594,30 @@
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
     </row>
-    <row r="45" spans="3:24" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="27"/>
-      <c r="E45" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
-      <c r="N45" s="39"/>
-      <c r="O45" s="39"/>
-      <c r="P45" s="39"/>
-      <c r="Q45" s="39"/>
-      <c r="R45" s="39"/>
-      <c r="S45" s="39"/>
-      <c r="T45" s="39"/>
-      <c r="U45" s="39"/>
-      <c r="V45" s="39"/>
-    </row>
-    <row r="46" spans="3:24" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:25" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="36"/>
+      <c r="E45" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="F45" s="41"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
+      <c r="K45" s="41"/>
+      <c r="L45" s="41"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="41"/>
+      <c r="O45" s="41"/>
+      <c r="P45" s="41"/>
+      <c r="Q45" s="41"/>
+      <c r="R45" s="41"/>
+      <c r="S45" s="41"/>
+      <c r="T45" s="41"/>
+      <c r="U45" s="41"/>
+      <c r="V45" s="41"/>
+    </row>
+    <row r="46" spans="3:25" ht="27.6" x14ac:dyDescent="0.25">
       <c r="C46" s="7" t="s">
         <v>34</v>
       </c>
@@ -3365,7 +3652,7 @@
         <v>17</v>
       </c>
       <c r="N46" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O46" s="8" t="s">
         <v>19</v>
@@ -3391,206 +3678,382 @@
       <c r="V46" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="W46" s="16"/>
+      <c r="W46" s="16" t="s">
+        <v>184</v>
+      </c>
       <c r="X46" s="16"/>
     </row>
-    <row r="47" spans="3:24" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="27" t="s">
+    <row r="47" spans="3:25" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="26"/>
-      <c r="E47" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>172</v>
+      <c r="D47" s="39"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="26" t="s">
+        <v>26</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
-      <c r="R47" s="2"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
-    </row>
-    <row r="48" spans="3:24" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-      <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-      <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
-    </row>
-    <row r="49" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
-    </row>
-    <row r="50" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-      <c r="U50" s="1"/>
-      <c r="V50" s="1"/>
-    </row>
-    <row r="51" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
-      <c r="Q51" s="2"/>
-      <c r="R51" s="2"/>
-      <c r="S51" s="1"/>
-      <c r="T51" s="1"/>
-      <c r="U51" s="1"/>
-      <c r="V51" s="1"/>
-    </row>
-    <row r="52" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="2"/>
-      <c r="S52" s="1"/>
-      <c r="T52" s="1"/>
-      <c r="U52" s="1"/>
-      <c r="V52" s="1"/>
-    </row>
-    <row r="53" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
-      <c r="R53" s="2"/>
-      <c r="S53" s="1"/>
-      <c r="T53" s="1"/>
-      <c r="U53" s="1"/>
-      <c r="V53" s="1"/>
-    </row>
-    <row r="54" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
-      <c r="S54" s="1"/>
-      <c r="T54" s="1"/>
-      <c r="U54" s="1"/>
-      <c r="V54" s="1"/>
-    </row>
-    <row r="55" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C55" s="27"/>
-      <c r="D55" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="E55" s="16"/>
+        <v>70</v>
+      </c>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="N47" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O47" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="P47" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q47" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="R47" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="S47" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="T47" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="U47" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="V47" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="W47" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="X47" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y47" s="32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="3:25" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="36"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="F48" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="M48" s="33"/>
+      <c r="N48" s="33"/>
+      <c r="O48" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="P48" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q48" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="R48" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="S48" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="T48" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="U48" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="V48" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="W48" s="19"/>
+      <c r="X48" s="35"/>
+      <c r="Y48" s="35"/>
+    </row>
+    <row r="49" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="36"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="36"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="36"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="P49" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q49" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="R49" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="S49" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="T49" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="U49" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="V49" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="36"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="36"/>
+      <c r="M50" s="31"/>
+      <c r="N50" s="31"/>
+      <c r="O50" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="P50" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q50" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="R50" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="S50" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="T50" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="U50" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="V50" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="36"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="G51" s="36"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="36"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="36"/>
+      <c r="M51" s="31"/>
+      <c r="N51" s="31"/>
+      <c r="O51" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="P51" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q51" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="R51" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="S51" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="T51" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="U51" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="V51" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="36"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="G52" s="36"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="31"/>
+      <c r="N52" s="31"/>
+      <c r="O52" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="P52" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q52" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="R52" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="S52" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="T52" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="U52" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="V52" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="36"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="F53" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G53" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="H53" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="I53" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="J53" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="K53" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="L53" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="M53" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="N53" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="O53" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="P53" s="33"/>
+      <c r="Q53" s="33"/>
+      <c r="R53" s="33"/>
+      <c r="S53" s="33"/>
+      <c r="T53" s="33"/>
+      <c r="U53" s="33"/>
+      <c r="V53" s="33"/>
+    </row>
+    <row r="54" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="36"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="F54" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G54" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="31"/>
+      <c r="L54" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="M54" s="31"/>
+      <c r="N54" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="O54" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="P54" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q54" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="R54" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="S54" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="T54" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="U54" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="V54" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="16" t="s">
+        <v>187</v>
+      </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
+      <c r="L55" s="33" t="s">
+        <v>228</v>
+      </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -3602,30 +4065,36 @@
       <c r="U55" s="1"/>
       <c r="V55" s="1"/>
     </row>
-    <row r="56" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
-      <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
-      <c r="Q56" s="2"/>
-      <c r="R56" s="2"/>
+    <row r="56" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F56" s="30"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="30"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="30"/>
+      <c r="K56" s="30"/>
+      <c r="L56" s="30"/>
+      <c r="M56" s="30"/>
+      <c r="N56" s="30"/>
+      <c r="O56" s="30"/>
+      <c r="P56" s="30"/>
+      <c r="Q56" s="30"/>
+      <c r="R56" s="30"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
     </row>
-    <row r="57" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E57" s="1"/>
+    <row r="57" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="16" t="s">
+        <v>204</v>
+      </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -3644,8 +4113,12 @@
       <c r="U57" s="1"/>
       <c r="V57" s="1"/>
     </row>
-    <row r="58" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E58" s="1"/>
+    <row r="58" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="16" t="s">
+        <v>206</v>
+      </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -3664,35 +4137,67 @@
       <c r="U58" s="1"/>
       <c r="V58" s="1"/>
     </row>
-    <row r="59" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="36"/>
+      <c r="D59" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="E59" s="1"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
-      <c r="S59" s="1"/>
-      <c r="T59" s="1"/>
-      <c r="U59" s="1"/>
-      <c r="V59" s="1"/>
-    </row>
-    <row r="60" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E60" s="1"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="33"/>
+      <c r="K59" s="33"/>
+      <c r="L59" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="M59" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="N59" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="O59" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P59" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q59" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="R59" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="S59" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T59" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="U59" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="V59" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="16" t="s">
+        <v>231</v>
+      </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
+      <c r="L60" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -3704,8 +4209,10 @@
       <c r="U60" s="1"/>
       <c r="V60" s="1"/>
     </row>
-    <row r="61" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E61" s="1"/>
+    <row r="61" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="36"/>
+      <c r="D61" s="36"/>
+      <c r="E61" s="16"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -3724,8 +4231,10 @@
       <c r="U61" s="1"/>
       <c r="V61" s="1"/>
     </row>
-    <row r="62" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E62" s="1"/>
+    <row r="62" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="16"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -3744,215 +4253,923 @@
       <c r="U62" s="1"/>
       <c r="V62" s="1"/>
     </row>
-    <row r="63" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="36"/>
+      <c r="D63" s="30"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
-      <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
-      <c r="P63" s="2"/>
-      <c r="Q63" s="2"/>
-      <c r="R63" s="2"/>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1"/>
-      <c r="U63" s="1"/>
-      <c r="V63" s="1"/>
-    </row>
-    <row r="64" spans="3:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F63" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G63" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="H63" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I63" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="J63" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K63" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L63" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="M63" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="N63" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="O63" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P63" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q63" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="R63" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="S63" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T63" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="U63" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="V63" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="W63" s="27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="64" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="36"/>
+      <c r="D64" s="33"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
-      <c r="O64" s="2"/>
-      <c r="P64" s="2"/>
-      <c r="Q64" s="2"/>
-      <c r="R64" s="2"/>
-      <c r="S64" s="1"/>
-      <c r="T64" s="1"/>
-      <c r="U64" s="1"/>
-      <c r="V64" s="1"/>
-    </row>
-    <row r="65" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F64" s="33"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="33"/>
+      <c r="M64" s="33"/>
+      <c r="N64" s="33"/>
+      <c r="O64" s="33"/>
+      <c r="P64" s="33"/>
+      <c r="Q64" s="33"/>
+      <c r="R64" s="33"/>
+      <c r="S64" s="33"/>
+      <c r="T64" s="33"/>
+      <c r="U64" s="33"/>
+      <c r="V64" s="33"/>
+      <c r="W64" s="35"/>
+    </row>
+    <row r="65" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="36"/>
+      <c r="D65" s="33"/>
       <c r="E65" s="1"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
-      <c r="M65" s="2"/>
-      <c r="N65" s="2"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="2"/>
-      <c r="S65" s="1"/>
-      <c r="T65" s="1"/>
-      <c r="U65" s="1"/>
-      <c r="V65" s="1"/>
-    </row>
-    <row r="66" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E66" s="1"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2"/>
-      <c r="N66" s="2"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
-      <c r="R66" s="2"/>
-      <c r="S66" s="1"/>
-      <c r="T66" s="1"/>
-      <c r="U66" s="1"/>
-      <c r="V66" s="1"/>
-    </row>
-    <row r="67" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E67" s="1"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="2"/>
-      <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="33"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="33"/>
+      <c r="K65" s="33"/>
+      <c r="L65" s="33"/>
+      <c r="M65" s="33"/>
+      <c r="N65" s="33"/>
+      <c r="O65" s="33"/>
+      <c r="P65" s="33"/>
+      <c r="Q65" s="33"/>
+      <c r="R65" s="33"/>
+      <c r="S65" s="33"/>
+      <c r="T65" s="33"/>
+      <c r="U65" s="33"/>
+      <c r="V65" s="33"/>
+      <c r="W65" s="35"/>
+    </row>
+    <row r="66" spans="3:23" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C66" s="36"/>
+      <c r="D66" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="E66" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="F66" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="H66" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="I66" s="39"/>
+      <c r="J66" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="K66" s="39"/>
+      <c r="L66" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="M66" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="N66" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="O66" s="30"/>
+      <c r="P66" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q66" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="R66" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="S66" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="T66" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="U66" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="V66" s="30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="67" spans="3:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="36"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="43" t="s">
+        <v>216</v>
+      </c>
+      <c r="G67" s="44"/>
+      <c r="H67" s="44"/>
+      <c r="I67" s="44"/>
+      <c r="J67" s="44"/>
+      <c r="K67" s="45"/>
+      <c r="L67" s="30"/>
+      <c r="M67" s="30"/>
+      <c r="N67" s="30"/>
+      <c r="O67" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="P67" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q67" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="R67" s="36"/>
+      <c r="S67" s="36"/>
+      <c r="T67" s="30" t="s">
+        <v>193</v>
+      </c>
       <c r="U67" s="1"/>
       <c r="V67" s="1"/>
     </row>
-    <row r="68" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E68" s="1"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
-      <c r="L68" s="2"/>
-      <c r="M68" s="2"/>
-      <c r="N68" s="2"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="2"/>
-      <c r="S68" s="1"/>
-      <c r="T68" s="1"/>
+    <row r="68" spans="3:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C68" s="36"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="40"/>
+      <c r="F68" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="G68" s="36"/>
+      <c r="H68" s="36"/>
+      <c r="I68" s="36"/>
+      <c r="J68" s="36"/>
+      <c r="K68" s="36"/>
+      <c r="L68" s="30"/>
+      <c r="M68" s="30"/>
+      <c r="N68" s="30"/>
+      <c r="O68" s="30"/>
+      <c r="P68" s="29"/>
+      <c r="Q68" s="30"/>
+      <c r="R68" s="30"/>
+      <c r="S68" s="30"/>
+      <c r="T68" s="30"/>
       <c r="U68" s="1"/>
       <c r="V68" s="1"/>
     </row>
-    <row r="69" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E69" s="1"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-      <c r="K69" s="2"/>
-      <c r="L69" s="2"/>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="2"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="1"/>
+    <row r="69" spans="3:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="36"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="40"/>
+      <c r="F69" s="36" t="s">
+        <v>197</v>
+      </c>
+      <c r="G69" s="36"/>
+      <c r="H69" s="36"/>
+      <c r="I69" s="36"/>
+      <c r="J69" s="36"/>
+      <c r="K69" s="36"/>
+      <c r="L69" s="30"/>
+      <c r="M69" s="30"/>
+      <c r="N69" s="30"/>
+      <c r="O69" s="30"/>
+      <c r="P69" s="29"/>
+      <c r="Q69" s="30"/>
+      <c r="R69" s="30"/>
+      <c r="S69" s="30"/>
+      <c r="T69" s="30"/>
       <c r="U69" s="1"/>
       <c r="V69" s="1"/>
     </row>
-    <row r="70" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-      <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
-      <c r="N70" s="3"/>
-    </row>
-    <row r="71" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
-      <c r="M71" s="3"/>
-      <c r="N71" s="3"/>
-    </row>
-    <row r="72" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
-      <c r="M72" s="3"/>
-      <c r="N72" s="3"/>
-    </row>
-    <row r="73" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="3"/>
-      <c r="L73" s="3"/>
-      <c r="M73" s="3"/>
-      <c r="N73" s="3"/>
-    </row>
-    <row r="74" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
-      <c r="M74" s="3"/>
-      <c r="N74" s="3"/>
-    </row>
-    <row r="75" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
-      <c r="M75" s="3"/>
-      <c r="N75" s="3"/>
+    <row r="70" spans="3:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="36"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="40"/>
+      <c r="F70" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="G70" s="36"/>
+      <c r="H70" s="36"/>
+      <c r="I70" s="36"/>
+      <c r="J70" s="36"/>
+      <c r="K70" s="36"/>
+      <c r="L70" s="30"/>
+      <c r="M70" s="30"/>
+      <c r="N70" s="30"/>
+      <c r="O70" s="30"/>
+      <c r="P70" s="29"/>
+      <c r="Q70" s="30"/>
+      <c r="R70" s="30"/>
+      <c r="S70" s="30"/>
+      <c r="T70" s="30"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+    </row>
+    <row r="71" spans="3:23" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="36"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="40"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="30"/>
+      <c r="I71" s="30"/>
+      <c r="J71" s="30"/>
+      <c r="K71" s="30"/>
+      <c r="L71" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="M71" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="N71" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="O71" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P71" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q71" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="R71" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="S71" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T71" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="U71" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="V71" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="36"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="G72" s="36"/>
+      <c r="H72" s="36"/>
+      <c r="I72" s="36"/>
+      <c r="J72" s="36"/>
+      <c r="K72" s="36"/>
+      <c r="L72" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="M72" s="30"/>
+      <c r="N72" s="30"/>
+      <c r="O72" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="P72" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q72" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="R72" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="S72" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="T72" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="U72" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="V72" s="30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="73" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="36"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="40"/>
+      <c r="F73" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="G73" s="36"/>
+      <c r="H73" s="36"/>
+      <c r="I73" s="36"/>
+      <c r="J73" s="36"/>
+      <c r="K73" s="36"/>
+      <c r="L73" s="30"/>
+      <c r="M73" s="30"/>
+      <c r="N73" s="30"/>
+      <c r="O73" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="P73" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q73" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="R73" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="S73" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="T73" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="U73" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="V73" s="30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="36"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="40"/>
+      <c r="F74" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="G74" s="36"/>
+      <c r="H74" s="36"/>
+      <c r="I74" s="36"/>
+      <c r="J74" s="36"/>
+      <c r="K74" s="36"/>
+      <c r="L74" s="30"/>
+      <c r="M74" s="30"/>
+      <c r="N74" s="30"/>
+      <c r="O74" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="P74" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q74" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="R74" s="36"/>
+      <c r="S74" s="36"/>
+      <c r="T74" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="U74" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="V74" s="30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="3:23" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="36"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="40"/>
+      <c r="F75" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="G75" s="36"/>
+      <c r="H75" s="36"/>
+      <c r="I75" s="36"/>
+      <c r="J75" s="36"/>
+      <c r="K75" s="36"/>
+      <c r="L75" s="30"/>
+      <c r="M75" s="30"/>
+      <c r="N75" s="30"/>
+      <c r="O75" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="P75" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q75" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="R75" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="S75" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="T75" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="U75" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="V75" s="30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="36"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="F76" s="43" t="s">
+        <v>218</v>
+      </c>
+      <c r="G76" s="44"/>
+      <c r="H76" s="44"/>
+      <c r="I76" s="44"/>
+      <c r="J76" s="44"/>
+      <c r="K76" s="45"/>
+      <c r="L76" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="M76" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="N76" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="O76" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="P76" s="26"/>
+      <c r="Q76" s="26"/>
+      <c r="R76" s="26"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+    </row>
+    <row r="77" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="30"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="G77" s="36"/>
+      <c r="H77" s="36"/>
+      <c r="I77" s="36"/>
+      <c r="J77" s="36"/>
+      <c r="K77" s="36"/>
+      <c r="L77" s="30"/>
+      <c r="M77" s="30"/>
+      <c r="N77" s="30"/>
+      <c r="O77" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="P77" s="30"/>
+      <c r="Q77" s="30"/>
+      <c r="R77" s="30"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+    </row>
+    <row r="78" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="30"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="36"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="36"/>
+      <c r="I78" s="36"/>
+      <c r="J78" s="36"/>
+      <c r="K78" s="36"/>
+      <c r="L78" s="30"/>
+      <c r="M78" s="30"/>
+      <c r="N78" s="30"/>
+      <c r="O78" s="30"/>
+      <c r="P78" s="30"/>
+      <c r="Q78" s="30"/>
+      <c r="R78" s="30"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+    </row>
+    <row r="79" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="30"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="36"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="36"/>
+      <c r="I79" s="36"/>
+      <c r="J79" s="36"/>
+      <c r="K79" s="36"/>
+      <c r="L79" s="30"/>
+      <c r="M79" s="30"/>
+      <c r="N79" s="30"/>
+      <c r="O79" s="30"/>
+      <c r="P79" s="30"/>
+      <c r="Q79" s="30"/>
+      <c r="R79" s="30"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="1"/>
+      <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
+    </row>
+    <row r="80" spans="3:23" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E80" s="1"/>
+      <c r="F80" s="30"/>
+      <c r="G80" s="30"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="30"/>
+      <c r="J80" s="30"/>
+      <c r="K80" s="30"/>
+      <c r="L80" s="30"/>
+      <c r="M80" s="30"/>
+      <c r="N80" s="30"/>
+      <c r="O80" s="30"/>
+      <c r="P80" s="30"/>
+      <c r="Q80" s="29"/>
+      <c r="R80" s="30"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+    </row>
+    <row r="81" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E81" s="1"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+      <c r="M81" s="2"/>
+      <c r="N81" s="2"/>
+      <c r="O81" s="2"/>
+      <c r="P81" s="2"/>
+      <c r="Q81" s="2"/>
+      <c r="R81" s="2"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="1"/>
+      <c r="U81" s="1"/>
+      <c r="V81" s="1"/>
+    </row>
+    <row r="82" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E82" s="1"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
+      <c r="O82" s="2"/>
+      <c r="P82" s="2"/>
+      <c r="Q82" s="2"/>
+      <c r="R82" s="2"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="1"/>
+      <c r="U82" s="1"/>
+      <c r="V82" s="1"/>
+    </row>
+    <row r="83" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E83" s="1"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+      <c r="M83" s="2"/>
+      <c r="N83" s="2"/>
+      <c r="O83" s="2"/>
+      <c r="P83" s="2"/>
+      <c r="Q83" s="2"/>
+      <c r="R83" s="2"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="1"/>
+      <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+    </row>
+    <row r="84" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E84" s="1"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+      <c r="L84" s="2"/>
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
+      <c r="O84" s="2"/>
+      <c r="P84" s="2"/>
+      <c r="Q84" s="2"/>
+      <c r="R84" s="2"/>
+      <c r="S84" s="1"/>
+      <c r="T84" s="1"/>
+      <c r="U84" s="1"/>
+      <c r="V84" s="1"/>
+    </row>
+    <row r="85" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E85" s="1"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+      <c r="P85" s="2"/>
+      <c r="Q85" s="2"/>
+      <c r="R85" s="2"/>
+      <c r="S85" s="1"/>
+      <c r="T85" s="1"/>
+      <c r="U85" s="1"/>
+      <c r="V85" s="1"/>
+    </row>
+    <row r="86" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E86" s="1"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
+      <c r="O86" s="2"/>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="2"/>
+      <c r="R86" s="2"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="1"/>
+      <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
+    </row>
+    <row r="87" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E87" s="1"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" s="2"/>
+      <c r="P87" s="2"/>
+      <c r="Q87" s="2"/>
+      <c r="R87" s="2"/>
+      <c r="S87" s="1"/>
+      <c r="T87" s="1"/>
+      <c r="U87" s="1"/>
+      <c r="V87" s="1"/>
+    </row>
+    <row r="88" spans="5:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E88" s="1"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2"/>
+      <c r="K88" s="2"/>
+      <c r="L88" s="2"/>
+      <c r="M88" s="2"/>
+      <c r="N88" s="2"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="2"/>
+      <c r="S88" s="1"/>
+      <c r="T88" s="1"/>
+      <c r="U88" s="1"/>
+      <c r="V88" s="1"/>
+    </row>
+    <row r="89" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E89" s="1"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
+      <c r="L89" s="2"/>
+      <c r="M89" s="2"/>
+      <c r="N89" s="2"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
+      <c r="R89" s="2"/>
+      <c r="S89" s="1"/>
+      <c r="T89" s="1"/>
+      <c r="U89" s="1"/>
+      <c r="V89" s="1"/>
+    </row>
+    <row r="90" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E90" s="1"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
+      <c r="M90" s="2"/>
+      <c r="N90" s="2"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="2"/>
+      <c r="S90" s="1"/>
+      <c r="T90" s="1"/>
+      <c r="U90" s="1"/>
+      <c r="V90" s="1"/>
+    </row>
+    <row r="91" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E91" s="1"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
+      <c r="L91" s="2"/>
+      <c r="M91" s="2"/>
+      <c r="N91" s="2"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="2"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="1"/>
+      <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
+    </row>
+    <row r="92" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E92" s="1"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="2"/>
+      <c r="S92" s="1"/>
+      <c r="T92" s="1"/>
+      <c r="U92" s="1"/>
+      <c r="V92" s="1"/>
+    </row>
+    <row r="93" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="3"/>
+      <c r="M93" s="3"/>
+      <c r="N93" s="3"/>
+    </row>
+    <row r="94" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+      <c r="M94" s="3"/>
+      <c r="N94" s="3"/>
+    </row>
+    <row r="95" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
+      <c r="M95" s="3"/>
+      <c r="N95" s="3"/>
+    </row>
+    <row r="96" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="3"/>
+      <c r="N96" s="3"/>
+    </row>
+    <row r="97" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
+      <c r="K97" s="3"/>
+      <c r="L97" s="3"/>
+      <c r="M97" s="3"/>
+      <c r="N97" s="3"/>
+    </row>
+    <row r="98" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="3"/>
+      <c r="M98" s="3"/>
+      <c r="N98" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="E45:V45"/>
+  <mergeCells count="49">
+    <mergeCell ref="E48:E52"/>
+    <mergeCell ref="L48:L52"/>
+    <mergeCell ref="F49:K49"/>
+    <mergeCell ref="F50:K50"/>
+    <mergeCell ref="F51:K51"/>
+    <mergeCell ref="F52:K52"/>
+    <mergeCell ref="F48:K48"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="E66:E75"/>
+    <mergeCell ref="F73:K73"/>
+    <mergeCell ref="F74:K74"/>
+    <mergeCell ref="F75:K75"/>
+    <mergeCell ref="F69:K69"/>
+    <mergeCell ref="F70:K70"/>
+    <mergeCell ref="F76:K76"/>
+    <mergeCell ref="F79:K79"/>
+    <mergeCell ref="F77:K77"/>
+    <mergeCell ref="F78:K78"/>
+    <mergeCell ref="F68:K68"/>
     <mergeCell ref="C3:Y3"/>
     <mergeCell ref="Y4:Y6"/>
     <mergeCell ref="L12:V12"/>
@@ -3963,19 +5180,25 @@
     <mergeCell ref="C4:E5"/>
     <mergeCell ref="L5:V5"/>
     <mergeCell ref="L4:V4"/>
-    <mergeCell ref="D14:D34"/>
-    <mergeCell ref="D36:D41"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="F4:K4"/>
+    <mergeCell ref="C47:C76"/>
+    <mergeCell ref="C7:C41"/>
+    <mergeCell ref="C43:C45"/>
     <mergeCell ref="R38:V38"/>
     <mergeCell ref="R39:V39"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="C47:C56"/>
-    <mergeCell ref="C7:C41"/>
-    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="D47:D58"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E45:V45"/>
+    <mergeCell ref="D14:D34"/>
+    <mergeCell ref="D36:D41"/>
+    <mergeCell ref="F67:K67"/>
+    <mergeCell ref="F72:K72"/>
+    <mergeCell ref="Q67:S67"/>
+    <mergeCell ref="Q74:S74"/>
+    <mergeCell ref="D66:D79"/>
+    <mergeCell ref="E76:E79"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3998,10 +5221,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="54"/>
     </row>
     <row r="4" spans="3:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">

</xml_diff>